<commit_message>
finalise replacement of ods with xls
</commit_message>
<xml_diff>
--- a/lib/setup_emldb_crosswalks_master.xlsx
+++ b/lib/setup_emldb_crosswalks_master.xlsx
@@ -11,14 +11,14 @@
     <sheet name="masterb8" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">masterb8!$A$1:$R$127</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">masterb8!$A$1:$R$127</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="217">
   <si>
     <t>eml_module</t>
   </si>
@@ -74,6 +74,12 @@
     <t>constraint</t>
   </si>
   <si>
+    <t>eml_standard_link</t>
+  </si>
+  <si>
+    <t>lter_manual_page</t>
+  </si>
+  <si>
     <t>package</t>
   </si>
   <si>
@@ -143,6 +149,23 @@
     <t>AUTHENTY</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">https://knb.ecoinformatics.org/#external//emlparser/docs/eml-2.1.1/./eml-resource.html</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve">#creator</t>
+    </r>
+  </si>
+  <si>
+    <t>Page 8</t>
+  </si>
+  <si>
     <t>pubDate</t>
   </si>
   <si>
@@ -407,6 +430,12 @@
     <t>document_id</t>
   </si>
   <si>
+    <t>dataTable</t>
+  </si>
+  <si>
+    <t>entityDescription</t>
+  </si>
+  <si>
     <t>notes</t>
   </si>
   <si>
@@ -419,12 +448,6 @@
     <t>data_table</t>
   </si>
   <si>
-    <t>dataTable</t>
-  </si>
-  <si>
-    <t>entityDescription</t>
-  </si>
-  <si>
     <t>notes_issues</t>
   </si>
   <si>
@@ -617,7 +640,7 @@
     <t>PRODUCER</t>
   </si>
   <si>
-    <t>  db.dataset.metadataprovider.requires = [IS_EMAIL(), IS_NOT_IN_DB(db, 'dataset.metadataprovider')]</t>
+    <t>db.dataset.metadataprovider.requires = [IS_EMAIL(), IS_NOT_IN_DB(db, 'dataset.metadataprovider')]</t>
   </si>
   <si>
     <t>'PRODDATEDOC',</t>
@@ -666,9 +689,10 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -689,8 +713,16 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color rgb="000000FF"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -736,10 +768,11 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -753,36 +786,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R127"/>
+  <dimension ref="A1:T127"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A13" xSplit="0" ySplit="1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="L58" activeCellId="0" pane="bottomLeft" sqref="L58"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="O1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="O1" activeCellId="0" pane="topLeft" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.1725490196078"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.6196078431373"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="16.278431372549"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0078431372549"/>
-    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="11.5764705882353"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.3098039215686"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5764705882353"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2901960784314"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="16.3607843137255"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="16" min="14" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="17.4"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.6313725490196"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,157 +864,169 @@
       <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="4">
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="O5" s="0" t="str">
         <f aca="false">IF(P5="","",LOWER(C5))</f>
         <v>title</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q5" s="0" t="str">
         <f aca="false">IF(P5="","","Field('"&amp;O5&amp;"','"&amp;P5&amp;"'),")</f>
         <v>Field('title','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O6" s="0" t="str">
         <f aca="false">IF(P6="","",LOWER(C6))</f>
         <v>creator</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q6" s="0" t="str">
         <f aca="false">IF(P6="","","Field('"&amp;O6&amp;"','"&amp;P6&amp;"'),")</f>
         <v>Field('creator','string'),</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="7">
+      <c r="S6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O7" s="0" t="str">
         <f aca="false">IF(P7="","",LOWER(C7))</f>
@@ -998,159 +1037,159 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="O8" s="0" t="str">
         <f aca="false">IF(P8="","",LOWER(C8))</f>
         <v>abstract</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q8" s="0" t="str">
         <f aca="false">IF(P8="","","Field('"&amp;O8&amp;"','"&amp;P8&amp;"'),")</f>
         <v>Field('abstract','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O9" s="0" t="str">
         <f aca="false">IF(P9="","",LOWER(C9))</f>
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J10" s="1"/>
       <c r="K10" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="O10" s="0" t="str">
         <f aca="false">IF(P10="","",LOWER(C10))</f>
         <v>intellectualrights</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q10" s="0" t="str">
         <f aca="false">IF(P10="","","Field('"&amp;O10&amp;"','"&amp;P10&amp;"'),")</f>
         <v>Field('intellectualrights','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H11" s="1"/>
       <c r="K11" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="O11" s="0" t="str">
         <f aca="false">IF(P11="","",LOWER(C11))</f>
         <v>contact</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q11" s="0" t="str">
         <f aca="false">IF(P11="","","Field('"&amp;O11&amp;"','"&amp;P11&amp;"'),")</f>
         <v>Field('contact','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="B12" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="H12" s="1"/>
       <c r="O12" s="0" t="str">
@@ -1162,24 +1201,24 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="13">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O13" s="0" t="str">
         <f aca="false">IF(P13="","",LOWER(C13))</f>
@@ -1190,55 +1229,55 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="14">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="14">
       <c r="A14" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="O14" s="0" t="str">
         <f aca="false">IF(P14="","",LOWER(C14))</f>
         <v>pubdate</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="Q14" s="0" t="str">
         <f aca="false">IF(P14="","","Field('"&amp;O14&amp;"','"&amp;P14&amp;"'),")</f>
         <v>Field('pubdate','date'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O15" s="0" t="str">
         <f aca="false">IF(P15="","",LOWER(C15))</f>
@@ -1249,21 +1288,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O16" s="0" t="str">
         <f aca="false">IF(P16="","",LOWER(C16))</f>
@@ -1274,21 +1313,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="17">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="17">
       <c r="A17" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O17" s="0" t="str">
         <f aca="false">IF(P17="","",LOWER(C17))</f>
@@ -1299,132 +1338,132 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="18">
       <c r="A18" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="O18" s="0" t="str">
         <f aca="false">IF(P18="","",LOWER(C18))</f>
         <v>geographicdescription</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q18" s="0" t="str">
         <f aca="false">IF(P18="","","Field('"&amp;O18&amp;"','"&amp;P18&amp;"'),")</f>
         <v>Field('geographicdescription','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="19">
       <c r="A19" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="O19" s="0" t="str">
         <f aca="false">IF(P19="","",LOWER(C19))</f>
         <v>boundingcoordinates</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q19" s="0" t="str">
         <f aca="false">IF(P19="","","Field('"&amp;O19&amp;"','"&amp;P19&amp;"'),")</f>
         <v>Field('boundingcoordinates','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="O20" s="0" t="str">
         <f aca="false">IF(P20="","",LOWER(C20))</f>
         <v>temporalcoverage</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q20" s="0" t="str">
         <f aca="false">IF(P20="","","Field('"&amp;O20&amp;"','"&amp;P20&amp;"'),")</f>
         <v>Field('temporalcoverage','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="21">
       <c r="B21" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="O21" s="0" t="str">
         <f aca="false">IF(P21="","",LOWER(C21))</f>
@@ -1435,18 +1474,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="22">
       <c r="B22" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O22" s="0" t="str">
         <f aca="false">IF(P22="","",LOWER(C22))</f>
@@ -1457,27 +1496,27 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="23">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="23">
       <c r="A23" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O23" s="0" t="str">
         <f aca="false">IF(P23="","",LOWER(C23))</f>
@@ -1488,27 +1527,27 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="24">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="24">
       <c r="A24" s="0" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O24" s="0" t="str">
         <f aca="false">IF(P24="","",LOWER(C24))</f>
@@ -1519,27 +1558,27 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="25">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="25">
       <c r="A25" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O25" s="0" t="str">
         <f aca="false">IF(P25="","",LOWER(C25))</f>
@@ -1550,24 +1589,24 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O26" s="0" t="str">
         <f aca="false">IF(P26="","",LOWER(C26))</f>
@@ -1578,27 +1617,27 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O27" s="0" t="str">
         <f aca="false">IF(P27="","",LOWER(C27))</f>
@@ -1609,16 +1648,16 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I28" s="1"/>
       <c r="K28" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O28" s="0" t="str">
         <f aca="false">IF(P28="","",LOWER(C28))</f>
@@ -1629,21 +1668,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O29" s="0" t="str">
         <f aca="false">IF(P29="","",LOWER(C29))</f>
@@ -1654,21 +1693,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O30" s="0" t="str">
         <f aca="false">IF(P30="","",LOWER(C30))</f>
@@ -1679,21 +1718,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O31" s="0" t="str">
         <f aca="false">IF(P31="","",LOWER(C31))</f>
@@ -1704,21 +1743,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K32" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O32" s="0" t="str">
         <f aca="false">IF(P32="","",LOWER(C32))</f>
@@ -1729,21 +1768,21 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O33" s="0" t="str">
         <f aca="false">IF(P33="","",LOWER(C33))</f>
@@ -1754,24 +1793,24 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K34" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="O34" s="0" t="str">
         <f aca="false">IF(P34="","",LOWER(C34))</f>
@@ -1782,18 +1821,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="O35" s="0" t="str">
         <f aca="false">IF(P35="","",LOWER(C35))</f>
@@ -1804,15 +1843,15 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="36">
       <c r="F36" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O36" s="0" t="str">
         <f aca="false">IF(P36="","",LOWER(C36))</f>
@@ -1823,12 +1862,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="37">
       <c r="F37" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="O37" s="0" t="str">
         <f aca="false">IF(P37="","",LOWER(C37))</f>
@@ -1839,12 +1878,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="38">
       <c r="F38" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="O38" s="0" t="str">
         <f aca="false">IF(P38="","",LOWER(C38))</f>
@@ -1855,74 +1894,74 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="G39" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="O39" s="0" t="str">
         <f aca="false">IF(P39="","",LOWER(C39))</f>
         <v>title</v>
       </c>
       <c r="P39" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q39" s="0" t="str">
         <f aca="false">IF(P39="","","Field('"&amp;O39&amp;"','"&amp;P39&amp;"'),")</f>
         <v>Field('title','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F40" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O40" s="0" t="str">
         <f aca="false">IF(P40="","",LOWER(C40))</f>
         <v>personnel</v>
       </c>
       <c r="P40" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q40" s="0" t="str">
         <f aca="false">IF(P40="","","Field('"&amp;O40&amp;"','"&amp;P40&amp;"'),")</f>
         <v>Field('personnel','string'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="F41" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O41" s="0" t="str">
         <f aca="false">IF(P41="","",LOWER(C41))</f>
@@ -1933,49 +1972,49 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B42" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O42" s="0" t="str">
         <f aca="false">IF(P42="","",LOWER(C42))</f>
         <v>abstract</v>
       </c>
       <c r="P42" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="Q42" s="0" t="str">
         <f aca="false">IF(P42="","","Field('"&amp;O42&amp;"','"&amp;P42&amp;"'),")</f>
         <v>Field('abstract','text'),</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="O43" s="0" t="str">
         <f aca="false">IF(P43="","",LOWER(C43))</f>
@@ -1986,18 +2025,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="F44" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O44" s="0" t="str">
         <f aca="false">IF(P44="","",LOWER(C44))</f>
@@ -2008,18 +2047,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B45" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>118</v>
-      </c>
-      <c r="F45" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O45" s="0" t="str">
         <f aca="false">IF(P45="","",LOWER(C45))</f>
@@ -2030,18 +2069,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B46" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F46" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="F46" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O46" s="0" t="str">
         <f aca="false">IF(P46="","",LOWER(C46))</f>
@@ -2052,18 +2091,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B47" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="F47" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="F47" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O47" s="0" t="str">
         <f aca="false">IF(P47="","",LOWER(C47))</f>
@@ -2074,18 +2113,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B48" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="F48" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="F48" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O48" s="0" t="str">
         <f aca="false">IF(P48="","",LOWER(C48))</f>
@@ -2096,18 +2135,18 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B49" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="F49" s="0" t="s">
-        <v>107</v>
       </c>
       <c r="O49" s="0" t="str">
         <f aca="false">IF(P49="","",LOWER(C49))</f>
@@ -2118,12 +2157,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="F50" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="H50" s="1"/>
       <c r="O50" s="0" t="str">
@@ -2135,16 +2174,16 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="51">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="51">
       <c r="F51" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="O51" s="0" t="str">
         <f aca="false">IF(P51="","",LOWER(C51))</f>
@@ -2155,16 +2194,16 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="F52" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="O52" s="0" t="str">
         <f aca="false">IF(P52="","",LOWER(C52))</f>
@@ -2175,16 +2214,16 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="53">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="53">
       <c r="F53" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H53" s="1"/>
       <c r="I53" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="O53" s="0" t="str">
         <f aca="false">IF(P53="","",LOWER(C53))</f>
@@ -2195,33 +2234,45 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
+      <c r="A54" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>134</v>
+      </c>
       <c r="F54" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="H54" s="1"/>
       <c r="O54" s="0" t="str">
         <f aca="false">IF(P54="","",LOWER(C54))</f>
-        <v/>
+        <v>entitydescription</v>
+      </c>
+      <c r="P54" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="Q54" s="0" t="str">
         <f aca="false">IF(P54="","","Field('"&amp;O54&amp;"','"&amp;P54&amp;"'),")</f>
-        <v/>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
+        <v>Field('entitydescription','string'),</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
       <c r="F55" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="O55" s="0" t="str">
         <f aca="false">IF(P55="","",LOWER(C55))</f>
@@ -2232,7 +2283,7 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="G56" s="2"/>
       <c r="H56" s="1"/>
       <c r="O56" s="0" t="str">
@@ -2244,12 +2295,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="F57" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H57" s="1"/>
       <c r="O57" s="0" t="str">
@@ -2261,47 +2312,40 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="58">
-      <c r="A58" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>133</v>
-      </c>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="58">
       <c r="C58" s="0" t="s">
-        <v>134</v>
+        <v>46</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="L58" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="O58" s="0" t="str">
-        <f aca="false">IF(P58="","",LOWER(C58))</f>
-        <v>entitydescription</v>
+        <v>141</v>
+      </c>
+      <c r="O58" s="0" t="s">
+        <v>139</v>
       </c>
       <c r="P58" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q58" s="0" t="str">
         <f aca="false">IF(P58="","","Field('"&amp;O58&amp;"','"&amp;P58&amp;"'),")</f>
-        <v>Field('entitydescription','string'),</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+        <v>Field('notes_issues','string'),</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
       <c r="F59" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H59" s="1"/>
       <c r="O59" s="0" t="str">
@@ -2313,12 +2357,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="60">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="60">
       <c r="F60" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H60" s="1"/>
       <c r="O60" s="0" t="str">
@@ -2330,12 +2374,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="F61" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="O61" s="0" t="str">
         <f aca="false">IF(P61="","",LOWER(C61))</f>
@@ -2346,12 +2390,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="62">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="62">
       <c r="F62" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="O62" s="0" t="str">
         <f aca="false">IF(P62="","",LOWER(C62))</f>
@@ -2362,15 +2406,15 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="63">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="63">
       <c r="F63" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="O63" s="0" t="str">
         <f aca="false">IF(P63="","",LOWER(C63))</f>
@@ -2381,12 +2425,12 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="64">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="64">
       <c r="F64" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="O64" s="0" t="str">
         <f aca="false">IF(P64="","",LOWER(C64))</f>
@@ -2397,503 +2441,503 @@
         <v/>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="F65" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="O65" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="O65" s="0" t="str">
         <f aca="false">IF(P65="","",LOWER(C65))</f>
-        <v>0</v>
-      </c>
-      <c r="Q65" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q65" s="0" t="str">
         <f aca="false">IF(P65="","","Field('"&amp;O65&amp;"','"&amp;P65&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="F66" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="K66" s="1"/>
-      <c r="O66" s="0" t="n">
+      <c r="O66" s="0" t="str">
         <f aca="false">IF(P66="","",LOWER(C66))</f>
-        <v>0</v>
-      </c>
-      <c r="Q66" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q66" s="0" t="str">
         <f aca="false">IF(P66="","","Field('"&amp;O66&amp;"','"&amp;P66&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="67">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="67">
       <c r="F67" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
-      <c r="O67" s="0" t="n">
+      <c r="O67" s="0" t="str">
         <f aca="false">IF(P67="","",LOWER(C67))</f>
-        <v>0</v>
-      </c>
-      <c r="Q67" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q67" s="0" t="str">
         <f aca="false">IF(P67="","","Field('"&amp;O67&amp;"','"&amp;P67&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="68">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="68">
       <c r="F68" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="K68" s="1"/>
-      <c r="O68" s="0" t="n">
+      <c r="O68" s="0" t="str">
         <f aca="false">IF(P68="","",LOWER(C68))</f>
-        <v>0</v>
-      </c>
-      <c r="Q68" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q68" s="0" t="str">
         <f aca="false">IF(P68="","","Field('"&amp;O68&amp;"','"&amp;P68&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="F69" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="K69" s="1"/>
-      <c r="O69" s="0" t="n">
+      <c r="O69" s="0" t="str">
         <f aca="false">IF(P69="","",LOWER(C69))</f>
-        <v>0</v>
-      </c>
-      <c r="Q69" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q69" s="0" t="str">
         <f aca="false">IF(P69="","","Field('"&amp;O69&amp;"','"&amp;P69&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="F70" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O70" s="0" t="n">
+        <v>157</v>
+      </c>
+      <c r="O70" s="0" t="str">
         <f aca="false">IF(P70="","",LOWER(C70))</f>
-        <v>0</v>
-      </c>
-      <c r="Q70" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q70" s="0" t="str">
         <f aca="false">IF(P70="","","Field('"&amp;O70&amp;"','"&amp;P70&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
       <c r="F71" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="O71" s="0" t="n">
+        <v>158</v>
+      </c>
+      <c r="O71" s="0" t="str">
         <f aca="false">IF(P71="","",LOWER(C71))</f>
-        <v>0</v>
-      </c>
-      <c r="Q71" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q71" s="0" t="str">
         <f aca="false">IF(P71="","","Field('"&amp;O71&amp;"','"&amp;P71&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="F72" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="O72" s="0" t="n">
+        <v>159</v>
+      </c>
+      <c r="O72" s="0" t="str">
         <f aca="false">IF(P72="","",LOWER(C72))</f>
-        <v>0</v>
-      </c>
-      <c r="Q72" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q72" s="0" t="str">
         <f aca="false">IF(P72="","","Field('"&amp;O72&amp;"','"&amp;P72&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="73">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="73">
       <c r="F73" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="O73" s="0" t="n">
+        <v>160</v>
+      </c>
+      <c r="O73" s="0" t="str">
         <f aca="false">IF(P73="","",LOWER(C73))</f>
-        <v>0</v>
-      </c>
-      <c r="Q73" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q73" s="0" t="str">
         <f aca="false">IF(P73="","","Field('"&amp;O73&amp;"','"&amp;P73&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="74">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="74">
       <c r="F74" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="O74" s="0" t="n">
+        <v>161</v>
+      </c>
+      <c r="O74" s="0" t="str">
         <f aca="false">IF(P74="","",LOWER(C74))</f>
-        <v>0</v>
-      </c>
-      <c r="Q74" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q74" s="0" t="str">
         <f aca="false">IF(P74="","","Field('"&amp;O74&amp;"','"&amp;P74&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="75">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="75">
       <c r="F75" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="O75" s="0" t="n">
+        <v>163</v>
+      </c>
+      <c r="O75" s="0" t="str">
         <f aca="false">IF(P75="","",LOWER(C75))</f>
-        <v>0</v>
-      </c>
-      <c r="Q75" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q75" s="0" t="str">
         <f aca="false">IF(P75="","","Field('"&amp;O75&amp;"','"&amp;P75&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="76">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="76">
       <c r="F76" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="O76" s="0" t="n">
+        <v>164</v>
+      </c>
+      <c r="O76" s="0" t="str">
         <f aca="false">IF(P76="","",LOWER(C76))</f>
-        <v>0</v>
-      </c>
-      <c r="Q76" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q76" s="0" t="str">
         <f aca="false">IF(P76="","","Field('"&amp;O76&amp;"','"&amp;P76&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="77">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="77">
       <c r="F77" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="O77" s="0" t="n">
+        <v>165</v>
+      </c>
+      <c r="O77" s="0" t="str">
         <f aca="false">IF(P77="","",LOWER(C77))</f>
-        <v>0</v>
-      </c>
-      <c r="Q77" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q77" s="0" t="str">
         <f aca="false">IF(P77="","","Field('"&amp;O77&amp;"','"&amp;P77&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="78">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="78">
       <c r="F78" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="O78" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="O78" s="0" t="str">
         <f aca="false">IF(P78="","",LOWER(C78))</f>
-        <v>0</v>
-      </c>
-      <c r="Q78" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q78" s="0" t="str">
         <f aca="false">IF(P78="","","Field('"&amp;O78&amp;"','"&amp;P78&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="79">
       <c r="F79" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="I79" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="O79" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="O79" s="0" t="str">
         <f aca="false">IF(P79="","",LOWER(C79))</f>
-        <v>0</v>
-      </c>
-      <c r="Q79" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q79" s="0" t="str">
         <f aca="false">IF(P79="","","Field('"&amp;O79&amp;"','"&amp;P79&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="80">
       <c r="F80" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>164</v>
-      </c>
-      <c r="O80" s="0" t="n">
+        <v>168</v>
+      </c>
+      <c r="O80" s="0" t="str">
         <f aca="false">IF(P80="","",LOWER(C80))</f>
-        <v>0</v>
-      </c>
-      <c r="Q80" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q80" s="0" t="str">
         <f aca="false">IF(P80="","","Field('"&amp;O80&amp;"','"&amp;P80&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="81">
       <c r="F81" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="O81" s="0" t="n">
+        <v>169</v>
+      </c>
+      <c r="O81" s="0" t="str">
         <f aca="false">IF(P81="","",LOWER(C81))</f>
-        <v>0</v>
-      </c>
-      <c r="Q81" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q81" s="0" t="str">
         <f aca="false">IF(P81="","","Field('"&amp;O81&amp;"','"&amp;P81&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="82">
       <c r="F82" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="O82" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="O82" s="0" t="str">
         <f aca="false">IF(P82="","",LOWER(C82))</f>
-        <v>0</v>
-      </c>
-      <c r="Q82" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q82" s="0" t="str">
         <f aca="false">IF(P82="","","Field('"&amp;O82&amp;"','"&amp;P82&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="83">
       <c r="F83" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="O83" s="0" t="n">
+        <v>171</v>
+      </c>
+      <c r="O83" s="0" t="str">
         <f aca="false">IF(P83="","",LOWER(C83))</f>
-        <v>0</v>
-      </c>
-      <c r="Q83" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q83" s="0" t="str">
         <f aca="false">IF(P83="","","Field('"&amp;O83&amp;"','"&amp;P83&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="84">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="84">
       <c r="F84" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G84" s="0" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="I84" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K84" s="1"/>
+      <c r="O84" s="0" t="str">
+        <f aca="false">IF(P84="","",LOWER(C84))</f>
+        <v/>
+      </c>
+      <c r="Q84" s="0" t="str">
+        <f aca="false">IF(P84="","","Field('"&amp;O84&amp;"','"&amp;P84&amp;"'),")</f>
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="85">
+      <c r="F85" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="J84" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="K84" s="1"/>
-      <c r="O84" s="0" t="n">
-        <f aca="false">IF(P84="","",LOWER(C84))</f>
-        <v>0</v>
-      </c>
-      <c r="Q84" s="0" t="n">
-        <f aca="false">IF(P84="","","Field('"&amp;O84&amp;"','"&amp;P84&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
-      <c r="F85" s="0" t="s">
-        <v>49</v>
-      </c>
       <c r="G85" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="O85" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="O85" s="0" t="str">
         <f aca="false">IF(P85="","",LOWER(C85))</f>
-        <v>0</v>
-      </c>
-      <c r="Q85" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q85" s="0" t="str">
         <f aca="false">IF(P85="","","Field('"&amp;O85&amp;"','"&amp;P85&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="86">
       <c r="F86" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G86" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="O86" s="0" t="n">
+        <v>175</v>
+      </c>
+      <c r="O86" s="0" t="str">
         <f aca="false">IF(P86="","",LOWER(C86))</f>
-        <v>0</v>
-      </c>
-      <c r="Q86" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q86" s="0" t="str">
         <f aca="false">IF(P86="","","Field('"&amp;O86&amp;"','"&amp;P86&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="87">
       <c r="F87" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="O87" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="O87" s="0" t="str">
         <f aca="false">IF(P87="","",LOWER(C87))</f>
-        <v>0</v>
-      </c>
-      <c r="Q87" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q87" s="0" t="str">
         <f aca="false">IF(P87="","","Field('"&amp;O87&amp;"','"&amp;P87&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="88">
       <c r="F88" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G88" s="0" t="s">
-        <v>172</v>
-      </c>
-      <c r="O88" s="0" t="n">
+        <v>176</v>
+      </c>
+      <c r="O88" s="0" t="str">
         <f aca="false">IF(P88="","",LOWER(C88))</f>
-        <v>0</v>
-      </c>
-      <c r="Q88" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q88" s="0" t="str">
         <f aca="false">IF(P88="","","Field('"&amp;O88&amp;"','"&amp;P88&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="89">
       <c r="F89" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="O89" s="0" t="n">
+        <v>177</v>
+      </c>
+      <c r="O89" s="0" t="str">
         <f aca="false">IF(P89="","",LOWER(C89))</f>
-        <v>0</v>
-      </c>
-      <c r="Q89" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q89" s="0" t="str">
         <f aca="false">IF(P89="","","Field('"&amp;O89&amp;"','"&amp;P89&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="90">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="90">
       <c r="F90" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G90" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="O90" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="O90" s="0" t="str">
         <f aca="false">IF(P90="","",LOWER(C90))</f>
-        <v>0</v>
-      </c>
-      <c r="Q90" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q90" s="0" t="str">
         <f aca="false">IF(P90="","","Field('"&amp;O90&amp;"','"&amp;P90&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="91">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="91">
       <c r="F91" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="O91" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="O91" s="0" t="str">
         <f aca="false">IF(P91="","",LOWER(C91))</f>
-        <v>0</v>
-      </c>
-      <c r="Q91" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q91" s="0" t="str">
         <f aca="false">IF(P91="","","Field('"&amp;O91&amp;"','"&amp;P91&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="92">
       <c r="F92" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="J92" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="O92" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="O92" s="0" t="str">
         <f aca="false">IF(P92="","",LOWER(C92))</f>
-        <v>0</v>
-      </c>
-      <c r="Q92" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q92" s="0" t="str">
         <f aca="false">IF(P92="","","Field('"&amp;O92&amp;"','"&amp;P92&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="93">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
         <v>133</v>
       </c>
@@ -2901,525 +2945,527 @@
         <v>133</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="K93" s="1"/>
       <c r="L93" s="0" t="s">
-        <v>181</v>
-      </c>
-      <c r="O93" s="0" t="n">
+        <v>185</v>
+      </c>
+      <c r="O93" s="0" t="str">
         <f aca="false">IF(P93="","",LOWER(C93))</f>
-        <v>0</v>
+        <v>entityname</v>
       </c>
       <c r="P93" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q93" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q93" s="0" t="str">
         <f aca="false">IF(P93="","","Field('"&amp;O93&amp;"','"&amp;P93&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
+        <v>Field('entityname','string'),</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="94">
       <c r="F94" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="O94" s="0" t="n">
+        <v>186</v>
+      </c>
+      <c r="O94" s="0" t="str">
         <f aca="false">IF(P94="","",LOWER(C94))</f>
-        <v>0</v>
-      </c>
-      <c r="Q94" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q94" s="0" t="str">
         <f aca="false">IF(P94="","","Field('"&amp;O94&amp;"','"&amp;P94&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="95">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="95">
       <c r="F95" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="O95" s="0" t="n">
+        <v>188</v>
+      </c>
+      <c r="O95" s="0" t="str">
         <f aca="false">IF(P95="","",LOWER(C95))</f>
-        <v>0</v>
-      </c>
-      <c r="Q95" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q95" s="0" t="str">
         <f aca="false">IF(P95="","","Field('"&amp;O95&amp;"','"&amp;P95&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="96">
       <c r="F96" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="O96" s="0" t="n">
+        <v>189</v>
+      </c>
+      <c r="O96" s="0" t="str">
         <f aca="false">IF(P96="","",LOWER(C96))</f>
-        <v>0</v>
-      </c>
-      <c r="Q96" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q96" s="0" t="str">
         <f aca="false">IF(P96="","","Field('"&amp;O96&amp;"','"&amp;P96&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="97">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="97">
       <c r="F97" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G97" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J97" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="O97" s="0" t="n">
+        <v>192</v>
+      </c>
+      <c r="O97" s="0" t="str">
         <f aca="false">IF(P97="","",LOWER(C97))</f>
-        <v>0</v>
-      </c>
-      <c r="Q97" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q97" s="0" t="str">
         <f aca="false">IF(P97="","","Field('"&amp;O97&amp;"','"&amp;P97&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="98">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="98">
       <c r="F98" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G98" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="O98" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="O98" s="0" t="str">
         <f aca="false">IF(P98="","",LOWER(C98))</f>
-        <v>0</v>
-      </c>
-      <c r="Q98" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q98" s="0" t="str">
         <f aca="false">IF(P98="","","Field('"&amp;O98&amp;"','"&amp;P98&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="99">
       <c r="F99" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G99" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O99" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="O99" s="0" t="str">
         <f aca="false">IF(P99="","",LOWER(C99))</f>
-        <v>0</v>
-      </c>
-      <c r="Q99" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q99" s="0" t="str">
         <f aca="false">IF(P99="","","Field('"&amp;O99&amp;"','"&amp;P99&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="100">
       <c r="F100" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G100" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="O100" s="0" t="n">
+        <v>194</v>
+      </c>
+      <c r="O100" s="0" t="str">
         <f aca="false">IF(P100="","",LOWER(C100))</f>
-        <v>0</v>
-      </c>
-      <c r="Q100" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q100" s="0" t="str">
         <f aca="false">IF(P100="","","Field('"&amp;O100&amp;"','"&amp;P100&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="101">
       <c r="F101" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G101" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="O101" s="0" t="n">
+        <v>196</v>
+      </c>
+      <c r="O101" s="0" t="str">
         <f aca="false">IF(P101="","",LOWER(C101))</f>
-        <v>0</v>
-      </c>
-      <c r="Q101" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q101" s="0" t="str">
         <f aca="false">IF(P101="","","Field('"&amp;O101&amp;"','"&amp;P101&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="102">
       <c r="F102" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G102" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="O102" s="0" t="n">
+        <v>198</v>
+      </c>
+      <c r="O102" s="0" t="str">
         <f aca="false">IF(P102="","",LOWER(C102))</f>
-        <v>0</v>
-      </c>
-      <c r="Q102" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q102" s="0" t="str">
         <f aca="false">IF(P102="","","Field('"&amp;O102&amp;"','"&amp;P102&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="103">
       <c r="F103" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G103" s="0" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="I103" s="0" t="s">
-        <v>195</v>
-      </c>
-      <c r="O103" s="0" t="n">
+        <v>199</v>
+      </c>
+      <c r="O103" s="0" t="str">
         <f aca="false">IF(P103="","",LOWER(C103))</f>
-        <v>0</v>
-      </c>
-      <c r="Q103" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q103" s="0" t="str">
         <f aca="false">IF(P103="","","Field('"&amp;O103&amp;"','"&amp;P103&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="104">
       <c r="F104" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G104" s="0" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="I104" s="0" t="s">
-        <v>196</v>
-      </c>
-      <c r="O104" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="O104" s="0" t="str">
         <f aca="false">IF(P104="","",LOWER(C104))</f>
-        <v>0</v>
-      </c>
-      <c r="Q104" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q104" s="0" t="str">
         <f aca="false">IF(P104="","","Field('"&amp;O104&amp;"','"&amp;P104&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
-      <c r="O105" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="105">
+      <c r="O105" s="0" t="str">
         <f aca="false">IF(P105="","",LOWER(C105))</f>
-        <v>0</v>
-      </c>
-      <c r="Q105" s="0" t="n">
+        <v/>
+      </c>
+      <c r="Q105" s="0" t="str">
         <f aca="false">IF(P105="","","Field('"&amp;O105&amp;"','"&amp;P105&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="106">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="106">
       <c r="A106" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="K106" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L106" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="O106" s="0" t="n">
+        <v>202</v>
+      </c>
+      <c r="O106" s="0" t="str">
         <f aca="false">IF(P106="","",LOWER(C106))</f>
-        <v>0</v>
+        <v>metadataprovider</v>
       </c>
       <c r="P106" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q106" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q106" s="0" t="str">
         <f aca="false">IF(P106="","","Field('"&amp;O106&amp;"','"&amp;P106&amp;"'),")</f>
-        <v>0</v>
+        <v>Field('metadataprovider','string'),</v>
       </c>
       <c r="R106" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="107">
+        <v>203</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="107">
       <c r="K107" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L107" s="0" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="O107" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q107" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q107" s="0" t="str">
         <f aca="false">IF(P107="","","Field('"&amp;O107&amp;"','"&amp;P107&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="108">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="108">
       <c r="K108" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L108" s="0" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O108" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q108" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q108" s="0" t="str">
         <f aca="false">IF(P108="","","Field('"&amp;O108&amp;"','"&amp;P108&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="109">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="109">
       <c r="A109" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K109" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L109" s="0" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="O109" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q109" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q109" s="0" t="str">
         <f aca="false">IF(P109="","","Field('"&amp;O109&amp;"','"&amp;P109&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="110">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="110">
       <c r="K110" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L110" s="0" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="O110" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q110" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q110" s="0" t="str">
         <f aca="false">IF(P110="","","Field('"&amp;O110&amp;"','"&amp;P110&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="111">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="111">
       <c r="K111" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L111" s="0" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="O111" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q111" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q111" s="0" t="str">
         <f aca="false">IF(P111="","","Field('"&amp;O111&amp;"','"&amp;P111&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="112">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="112">
       <c r="K112" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L112" s="0" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="O112" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q112" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q112" s="0" t="str">
         <f aca="false">IF(P112="","","Field('"&amp;O112&amp;"','"&amp;P112&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="113">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="113">
       <c r="K113" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L113" s="0" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="O113" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q113" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q113" s="0" t="str">
         <f aca="false">IF(P113="","","Field('"&amp;O113&amp;"','"&amp;P113&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="114">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="114">
       <c r="K114" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L114" s="0" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="O114" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q114" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q114" s="0" t="str">
         <f aca="false">IF(P114="","","Field('"&amp;O114&amp;"','"&amp;P114&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="115">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="115">
       <c r="K115" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L115" s="0" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="O115" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q115" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q115" s="0" t="str">
         <f aca="false">IF(P115="","","Field('"&amp;O115&amp;"','"&amp;P115&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="116">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="116">
       <c r="K116" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L116" s="0" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="O116" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q116" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q116" s="0" t="str">
         <f aca="false">IF(P116="","","Field('"&amp;O116&amp;"','"&amp;P116&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="117">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="117">
       <c r="K117" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L117" s="0" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="O117" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P117" s="0" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q117" s="0" t="n">
+        <v>215</v>
+      </c>
+      <c r="Q117" s="0" t="str">
         <f aca="false">IF(P117="","","Field('"&amp;O117&amp;"','"&amp;P117&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="118">
+        <v>Field('NA','TODO'),</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="118">
       <c r="K118" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L118" s="0" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="O118" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q118" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q118" s="0" t="str">
         <f aca="false">IF(P118="","","Field('"&amp;O118&amp;"','"&amp;P118&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="119">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="119">
       <c r="K119" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O119" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q119" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="Q119" s="0" t="str">
         <f aca="false">IF(P119="","","Field('"&amp;O119&amp;"','"&amp;P119&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="120">
-      <c r="Q120" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="120">
+      <c r="Q120" s="0" t="str">
         <f aca="false">IF(P120="","","Field('"&amp;O120&amp;"','"&amp;P120&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="121">
-      <c r="Q121" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="121">
+      <c r="Q121" s="0" t="str">
         <f aca="false">IF(P121="","","Field('"&amp;O121&amp;"','"&amp;P121&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="122">
-      <c r="Q122" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="122">
+      <c r="Q122" s="0" t="str">
         <f aca="false">IF(P122="","","Field('"&amp;O122&amp;"','"&amp;P122&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="123">
-      <c r="Q123" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="123">
+      <c r="Q123" s="0" t="str">
         <f aca="false">IF(P123="","","Field('"&amp;O123&amp;"','"&amp;P123&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="124">
-      <c r="Q124" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="124">
+      <c r="Q124" s="0" t="str">
         <f aca="false">IF(P124="","","Field('"&amp;O124&amp;"','"&amp;P124&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="125">
-      <c r="Q125" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="125">
+      <c r="Q125" s="0" t="str">
         <f aca="false">IF(P125="","","Field('"&amp;O125&amp;"','"&amp;P125&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="126">
-      <c r="Q126" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="126">
+      <c r="Q126" s="0" t="str">
         <f aca="false">IF(P126="","","Field('"&amp;O126&amp;"','"&amp;P126&amp;"'),")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="127">
-      <c r="Q127" s="0" t="n">
+        <v/>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="127">
+      <c r="Q127" s="0" t="str">
         <f aca="false">IF(P127="","","Field('"&amp;O127&amp;"','"&amp;P127&amp;"'),")</f>
-        <v>0</v>
+        <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R127"/>
+  <hyperlinks>
+    <hyperlink display="https://knb.ecoinformatics.org/#external//emlparser/docs/eml-2.1.1/./eml-resource.html" location="external//emlparser/docs/eml-2.1.1/./eml-resource.html" ref="S6" r:id="rId1"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
@@ -3427,6 +3473,5 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>